<commit_message>
Updated value calculator spreadsheet to use last years best theoretical team total points as benchmark for valuing components
</commit_message>
<xml_diff>
--- a/Artifacts/component_valuer.xlsx
+++ b/Artifacts/component_valuer.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Haas F1 Team</t>
   </si>
@@ -96,15 +96,6 @@
     <t>Driver</t>
   </si>
   <si>
-    <t>Max Driver Cost</t>
-  </si>
-  <si>
-    <t>Max Car Cost</t>
-  </si>
-  <si>
-    <t>Max Engine Cost</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -151,6 +142,9 @@
   </si>
   <si>
     <t>Honda</t>
+  </si>
+  <si>
+    <t>Best Theoretical Team Last Year Points</t>
   </si>
 </sst>
 </file>
@@ -158,7 +152,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -197,16 +191,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,58 +504,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="F1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="1"/>
+      <c r="G1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -569,25 +566,27 @@
       <c r="C3">
         <v>12040</v>
       </c>
-      <c r="D3" s="4">
-        <f>C3/$C$3*$C$26</f>
-        <v>40</v>
-      </c>
-      <c r="F3">
+      <c r="D3" s="5">
+        <f>C3/$C$26%</f>
+        <v>37.865207409504038</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="5">
         <v>10802</v>
       </c>
-      <c r="I3" s="4">
-        <f>H3/$H$3*$C$27</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="5">
+        <f>I3/$C$26%</f>
+        <v>33.971758341981946</v>
+      </c>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -597,25 +596,27 @@
       <c r="C4">
         <v>11302</v>
       </c>
-      <c r="D4" s="4">
-        <f>C4/$C$3*$C$26</f>
-        <v>37.548172757475086</v>
-      </c>
-      <c r="F4">
+      <c r="D4" s="5">
+        <f t="shared" ref="D4:D24" si="0">C4/$C$26%</f>
+        <v>35.544233732742079</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4">
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="5">
         <v>7242</v>
       </c>
-      <c r="I4" s="4">
-        <f>H4/$H$3*$C$27</f>
-        <v>23.46509905573042</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="5">
+        <f t="shared" ref="J4:J13" si="1">I4/$C$26%</f>
+        <v>22.775733559769787</v>
+      </c>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -625,25 +626,27 @@
       <c r="C5">
         <v>8302</v>
       </c>
-      <c r="D5" s="4">
-        <f>C5/$C$3*$C$26</f>
-        <v>27.581395348837209</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="5">
+        <f t="shared" si="0"/>
+        <v>26.109381388181273</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5">
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="5">
         <v>6302</v>
       </c>
-      <c r="I5" s="4">
-        <f>H5/$H$3*$C$27</f>
-        <v>20.419366783928904</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="5">
+        <f t="shared" si="1"/>
+        <v>19.819479825140736</v>
+      </c>
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -653,25 +656,27 @@
       <c r="C6">
         <v>6962</v>
       </c>
-      <c r="D6" s="4">
-        <f>C6/$C$3*$C$26</f>
-        <v>23.129568106312291</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>21.895147340944114</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="G6">
         <v>4</v>
       </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6">
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="5">
         <v>4818</v>
       </c>
-      <c r="I6" s="4">
-        <f>H6/$H$3*$C$27</f>
-        <v>15.610997963340122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="5">
+        <f t="shared" si="1"/>
+        <v>15.152372865364656</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -681,25 +686,27 @@
       <c r="C7">
         <v>6796</v>
       </c>
-      <c r="D7" s="4">
-        <f>C7/$C$3*$C$26</f>
-        <v>22.578073089701</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>21.373085511211748</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="G7">
         <v>5</v>
       </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7">
+      <c r="H7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="5">
         <v>4542</v>
       </c>
-      <c r="I7" s="4">
-        <f>H7/$H$3*$C$27</f>
-        <v>14.716719126087762</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="5">
+        <f t="shared" si="1"/>
+        <v>14.284366449665061</v>
+      </c>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -709,25 +716,27 @@
       <c r="C8">
         <v>6354</v>
       </c>
-      <c r="D8" s="4">
-        <f>C8/$C$3*$C$26</f>
-        <v>21.109634551495017</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>19.98301726577979</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="G8">
         <v>6</v>
       </c>
-      <c r="G8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8">
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="5">
         <v>3546</v>
       </c>
-      <c r="I8" s="4">
-        <f>H8/$H$3*$C$27</f>
-        <v>11.489538974264024</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="5">
+        <f t="shared" si="1"/>
+        <v>11.151995471270874</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -737,25 +746,27 @@
       <c r="C9">
         <v>5072</v>
       </c>
-      <c r="D9" s="4">
-        <f>C9/$C$3*$C$26</f>
-        <v>16.85049833887043</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>15.951190363870804</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="G9">
         <v>7</v>
       </c>
-      <c r="G9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9">
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="5">
         <v>3514</v>
       </c>
-      <c r="I9" s="4">
-        <f>H9/$H$3*$C$27</f>
-        <v>11.385854471394186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="5">
+        <f t="shared" si="1"/>
+        <v>11.051357046262225</v>
+      </c>
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -765,25 +776,27 @@
       <c r="C10">
         <v>4740</v>
       </c>
-      <c r="D10" s="4">
-        <f>C10/$C$3*$C$26</f>
-        <v>15.747508305647841</v>
-      </c>
-      <c r="F10">
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
+        <v>14.907066704406075</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="G10">
         <v>8</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>0</v>
       </c>
-      <c r="H10">
+      <c r="I10" s="5">
         <v>3186</v>
       </c>
-      <c r="I10" s="4">
-        <f>H10/$H$3*$C$27</f>
-        <v>10.323088316978337</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="5">
+        <f t="shared" si="1"/>
+        <v>10.019813189923577</v>
+      </c>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -793,25 +806,27 @@
       <c r="C11">
         <v>4216</v>
       </c>
-      <c r="D11" s="4">
-        <f>C11/$C$3*$C$26</f>
-        <v>14.006644518272424</v>
-      </c>
-      <c r="F11">
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>13.259112494889454</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="G11">
         <v>9</v>
       </c>
-      <c r="G11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11">
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" s="5">
         <v>2598</v>
       </c>
-      <c r="I11" s="4">
-        <f>H11/$H$3*$C$27</f>
-        <v>8.4178855767450482</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="5">
+        <f t="shared" si="1"/>
+        <v>8.1705821303896595</v>
+      </c>
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -821,25 +836,27 @@
       <c r="C12">
         <v>3964</v>
       </c>
-      <c r="D12" s="4">
-        <f>C12/$C$3*$C$26</f>
-        <v>13.169435215946843</v>
-      </c>
-      <c r="F12">
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>12.466584897946346</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="G12">
         <v>10</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>1</v>
       </c>
-      <c r="H12">
+      <c r="I12" s="5">
         <v>2438</v>
       </c>
-      <c r="I12" s="4">
-        <f>H12/$H$3*$C$27</f>
-        <v>7.8994630623958519</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="5">
+        <f t="shared" si="1"/>
+        <v>7.6673900053464159</v>
+      </c>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -849,25 +866,27 @@
       <c r="C13">
         <v>3810</v>
       </c>
-      <c r="D13" s="4">
-        <f>C13/$C$3*$C$26</f>
-        <v>12.657807308970099</v>
-      </c>
-      <c r="F13">
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
+        <v>11.982262477592224</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="G13">
         <v>11</v>
       </c>
-      <c r="G13" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13">
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="5">
         <v>2242</v>
       </c>
-      <c r="I13" s="4">
-        <f>H13/$H$3*$C$27</f>
-        <v>7.264395482318089</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="5">
+        <f t="shared" si="1"/>
+        <v>7.0509796521684427</v>
+      </c>
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -877,13 +896,14 @@
       <c r="C14">
         <v>3644</v>
       </c>
-      <c r="D14" s="4">
-        <f>C14/$C$3*$C$26</f>
-        <v>12.106312292358803</v>
-      </c>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>11.46020064785986</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -893,13 +913,14 @@
       <c r="C15">
         <v>3126</v>
       </c>
-      <c r="D15" s="4">
-        <f>C15/$C$3*$C$26</f>
-        <v>10.385382059800666</v>
-      </c>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>9.8311161430323608</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -909,18 +930,19 @@
       <c r="C16">
         <v>3092</v>
       </c>
-      <c r="D16" s="4">
-        <f>C16/$C$3*$C$26</f>
-        <v>10.272425249169434</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>9.7241878164606721</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="G16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -930,53 +952,57 @@
       <c r="C17">
         <v>3052</v>
       </c>
-      <c r="D17" s="4">
-        <f>C17/$C$3*$C$26</f>
-        <v>10.13953488372093</v>
-      </c>
-      <c r="F17">
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>9.5983897851998616</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="G17">
         <v>1</v>
       </c>
-      <c r="G17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17">
+      <c r="H17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="5">
         <v>9552</v>
       </c>
-      <c r="I17" s="4">
-        <f>H17/$H$3*$C$28</f>
-        <v>26.528420662840215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="5">
+        <f t="shared" ref="J17:J20" si="2">I17/$C$26%</f>
+        <v>30.040569865081608</v>
+      </c>
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C18">
         <v>2736</v>
       </c>
-      <c r="D18" s="4">
-        <f>C18/$C$3*$C$26</f>
-        <v>9.0897009966777418</v>
-      </c>
-      <c r="F18">
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
+        <v>8.6045853382394561</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="G18">
         <v>2</v>
       </c>
-      <c r="G18" t="s">
-        <v>37</v>
-      </c>
-      <c r="H18">
+      <c r="H18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="5">
         <v>6420</v>
       </c>
-      <c r="I18" s="4">
-        <f>H18/$H$3*$C$28</f>
-        <v>17.830031475652657</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="5">
+        <f t="shared" si="2"/>
+        <v>20.190584017360127</v>
+      </c>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -986,25 +1012,27 @@
       <c r="C19">
         <v>2500</v>
       </c>
-      <c r="D19" s="4">
-        <f>C19/$C$3*$C$26</f>
-        <v>8.3056478405315612</v>
-      </c>
-      <c r="F19">
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
+        <v>7.8623769538006725</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="G19">
         <v>3</v>
       </c>
-      <c r="G19" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19">
+      <c r="H19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="5">
         <v>4170</v>
       </c>
-      <c r="I19" s="4">
-        <f>H19/$H$3*$C$28</f>
-        <v>11.581188668765042</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="5">
+        <f t="shared" si="2"/>
+        <v>13.114444758939522</v>
+      </c>
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1014,25 +1042,27 @@
       <c r="C20">
         <v>2196</v>
       </c>
-      <c r="D20" s="4">
-        <f>C20/$C$3*$C$26</f>
-        <v>7.2956810631229239</v>
-      </c>
-      <c r="F20">
+      <c r="D20" s="5">
+        <f t="shared" si="0"/>
+        <v>6.9063119162185105</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="G20">
         <v>4</v>
       </c>
-      <c r="G20" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20">
+      <c r="H20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="5">
         <v>1473</v>
       </c>
-      <c r="I20" s="4">
-        <f>H20/$H$3*$C$28</f>
-        <v>4.0909090909090908</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="5">
+        <f t="shared" si="2"/>
+        <v>4.632512501179356</v>
+      </c>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1042,29 +1072,35 @@
       <c r="C21">
         <v>2132</v>
       </c>
-      <c r="D21" s="4">
-        <f>C21/$C$3*$C$26</f>
-        <v>7.0830564784053154</v>
-      </c>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
+        <v>6.705035066201213</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C22">
         <v>2098</v>
       </c>
-      <c r="D22" s="4">
-        <f>C22/$C$3*$C$26</f>
-        <v>6.970099667774087</v>
-      </c>
-      <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>6.5981067396295243</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1074,67 +1110,51 @@
       <c r="C23">
         <v>1934</v>
       </c>
-      <c r="D23" s="4">
-        <f>C23/$C$3*$C$26</f>
-        <v>6.4252491694352152</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
+        <v>6.0823348114601998</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <v>1702</v>
       </c>
-      <c r="D24" s="4">
-        <f>C24/$C$3*$C$26</f>
-        <v>5.6544850498338874</v>
-      </c>
-      <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="3">
-        <v>40</v>
-      </c>
-      <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="3">
-        <v>35</v>
-      </c>
-      <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="3">
-        <v>30</v>
-      </c>
-      <c r="I28" s="4"/>
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
+        <v>5.3527062301474979</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="2">
+        <v>31797</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="F1:H1"/>
+  <mergeCells count="3">
+    <mergeCell ref="G1:I1"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="G16:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated 2017 costing data based off new calculator spreadsheet
</commit_message>
<xml_diff>
--- a/Artifacts/component_valuer.xlsx
+++ b/Artifacts/component_valuer.xlsx
@@ -566,7 +566,7 @@
       <c r="C3">
         <v>12040</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <f>C3/$C$26%</f>
         <v>37.865207409504038</v>
       </c>
@@ -580,7 +580,7 @@
       <c r="I3" s="5">
         <v>10802</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="3">
         <f>I3/$C$26%</f>
         <v>33.971758341981946</v>
       </c>
@@ -596,7 +596,7 @@
       <c r="C4">
         <v>11302</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <f t="shared" ref="D4:D24" si="0">C4/$C$26%</f>
         <v>35.544233732742079</v>
       </c>
@@ -610,7 +610,7 @@
       <c r="I4" s="5">
         <v>7242</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="3">
         <f t="shared" ref="J4:J13" si="1">I4/$C$26%</f>
         <v>22.775733559769787</v>
       </c>
@@ -626,7 +626,7 @@
       <c r="C5">
         <v>8302</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <f t="shared" si="0"/>
         <v>26.109381388181273</v>
       </c>
@@ -640,7 +640,7 @@
       <c r="I5" s="5">
         <v>6302</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="3">
         <f t="shared" si="1"/>
         <v>19.819479825140736</v>
       </c>
@@ -656,7 +656,7 @@
       <c r="C6">
         <v>6962</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>21.895147340944114</v>
       </c>
@@ -670,7 +670,7 @@
       <c r="I6" s="5">
         <v>4818</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="3">
         <f t="shared" si="1"/>
         <v>15.152372865364656</v>
       </c>
@@ -686,7 +686,7 @@
       <c r="C7">
         <v>6796</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
         <v>21.373085511211748</v>
       </c>
@@ -700,7 +700,7 @@
       <c r="I7" s="5">
         <v>4542</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="3">
         <f t="shared" si="1"/>
         <v>14.284366449665061</v>
       </c>
@@ -716,7 +716,7 @@
       <c r="C8">
         <v>6354</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>19.98301726577979</v>
       </c>
@@ -730,7 +730,7 @@
       <c r="I8" s="5">
         <v>3546</v>
       </c>
-      <c r="J8" s="5">
+      <c r="J8" s="3">
         <f t="shared" si="1"/>
         <v>11.151995471270874</v>
       </c>
@@ -746,7 +746,7 @@
       <c r="C9">
         <v>5072</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>15.951190363870804</v>
       </c>
@@ -760,7 +760,7 @@
       <c r="I9" s="5">
         <v>3514</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="3">
         <f t="shared" si="1"/>
         <v>11.051357046262225</v>
       </c>
@@ -776,7 +776,7 @@
       <c r="C10">
         <v>4740</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>14.907066704406075</v>
       </c>
@@ -790,7 +790,7 @@
       <c r="I10" s="5">
         <v>3186</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="3">
         <f t="shared" si="1"/>
         <v>10.019813189923577</v>
       </c>
@@ -806,7 +806,7 @@
       <c r="C11">
         <v>4216</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>13.259112494889454</v>
       </c>
@@ -820,7 +820,7 @@
       <c r="I11" s="5">
         <v>2598</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="3">
         <f t="shared" si="1"/>
         <v>8.1705821303896595</v>
       </c>
@@ -836,7 +836,7 @@
       <c r="C12">
         <v>3964</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>12.466584897946346</v>
       </c>
@@ -850,7 +850,7 @@
       <c r="I12" s="5">
         <v>2438</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="3">
         <f t="shared" si="1"/>
         <v>7.6673900053464159</v>
       </c>
@@ -866,7 +866,7 @@
       <c r="C13">
         <v>3810</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
         <v>11.982262477592224</v>
       </c>
@@ -880,7 +880,7 @@
       <c r="I13" s="5">
         <v>2242</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="3">
         <f t="shared" si="1"/>
         <v>7.0509796521684427</v>
       </c>
@@ -896,7 +896,7 @@
       <c r="C14">
         <v>3644</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="3">
         <f t="shared" si="0"/>
         <v>11.46020064785986</v>
       </c>
@@ -913,7 +913,7 @@
       <c r="C15">
         <v>3126</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="3">
         <f t="shared" si="0"/>
         <v>9.8311161430323608</v>
       </c>
@@ -930,7 +930,7 @@
       <c r="C16">
         <v>3092</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="3">
         <f t="shared" si="0"/>
         <v>9.7241878164606721</v>
       </c>
@@ -952,7 +952,7 @@
       <c r="C17">
         <v>3052</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="3">
         <f t="shared" si="0"/>
         <v>9.5983897851998616</v>
       </c>
@@ -966,7 +966,7 @@
       <c r="I17" s="5">
         <v>9552</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="3">
         <f t="shared" ref="J17:J20" si="2">I17/$C$26%</f>
         <v>30.040569865081608</v>
       </c>
@@ -982,7 +982,7 @@
       <c r="C18">
         <v>2736</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="3">
         <f t="shared" si="0"/>
         <v>8.6045853382394561</v>
       </c>
@@ -996,7 +996,7 @@
       <c r="I18" s="5">
         <v>6420</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="3">
         <f t="shared" si="2"/>
         <v>20.190584017360127</v>
       </c>
@@ -1012,7 +1012,7 @@
       <c r="C19">
         <v>2500</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="3">
         <f t="shared" si="0"/>
         <v>7.8623769538006725</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="I19" s="5">
         <v>4170</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19" s="3">
         <f t="shared" si="2"/>
         <v>13.114444758939522</v>
       </c>
@@ -1042,7 +1042,7 @@
       <c r="C20">
         <v>2196</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="3">
         <f t="shared" si="0"/>
         <v>6.9063119162185105</v>
       </c>
@@ -1056,7 +1056,7 @@
       <c r="I20" s="5">
         <v>1473</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20" s="3">
         <f t="shared" si="2"/>
         <v>4.632512501179356</v>
       </c>
@@ -1072,7 +1072,7 @@
       <c r="C21">
         <v>2132</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="3">
         <f t="shared" si="0"/>
         <v>6.705035066201213</v>
       </c>
@@ -1091,7 +1091,7 @@
       <c r="C22">
         <v>2098</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="3">
         <f t="shared" si="0"/>
         <v>6.5981067396295243</v>
       </c>
@@ -1110,7 +1110,7 @@
       <c r="C23">
         <v>1934</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="3">
         <f t="shared" si="0"/>
         <v>6.0823348114601998</v>
       </c>
@@ -1130,7 +1130,7 @@
       <c r="C24">
         <v>1702</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="3">
         <f t="shared" si="0"/>
         <v>5.3527062301474979</v>
       </c>

</xml_diff>